<commit_message>
Adding the jupyter notebooks and presentation folder
</commit_message>
<xml_diff>
--- a/Datasets/Employment in HTEC.xlsx
+++ b/Datasets/Employment in HTEC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibsi\Desktop\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibsi\Desktop\STEM-HTEC-Emplyoment-in-the-EU\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C3F8D4-36F7-4DA9-9377-136CE0DB3047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B837D4F-2E73-4854-B640-7FD13BD11FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="6" xr2:uid="{58E025E2-53D6-4113-B2BA-F8E123B61C13}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="&lt;Secondary (thousands)" sheetId="3" r:id="rId2"/>
     <sheet name="&lt;Tertirary (thousands)" sheetId="4" r:id="rId3"/>
     <sheet name="Tertiary (thousands)" sheetId="5" r:id="rId4"/>
-    <sheet name="&lt;Secondary (%)" sheetId="8" r:id="rId5"/>
-    <sheet name="&lt;Tertirary(%)" sheetId="9" r:id="rId6"/>
+    <sheet name="&lt;Secondary(%)" sheetId="8" r:id="rId5"/>
+    <sheet name="&lt;Tertiary(%)" sheetId="9" r:id="rId6"/>
     <sheet name="Tertiary(%)" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="51">
-  <si>
-    <t>GEO/TIME</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="52">
   <si>
     <t>2010</t>
   </si>
@@ -193,13 +190,19 @@
   <si>
     <t>Turkey</t>
   </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -266,7 +269,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -586,7 +589,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="A42:C43"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -597,42 +600,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>6887</v>
@@ -667,7 +670,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>8102.6</v>
@@ -702,7 +705,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>6777.9</v>
@@ -737,7 +740,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>5423.2</v>
@@ -772,7 +775,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>211.2</v>
@@ -807,7 +810,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>93.3</v>
@@ -842,7 +845,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4">
         <v>209.4</v>
@@ -877,7 +880,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
         <v>144.6</v>
@@ -912,7 +915,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4">
         <v>1627.8</v>
@@ -947,7 +950,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4">
         <v>19.5</v>
@@ -982,7 +985,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>146.9</v>
@@ -1017,7 +1020,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4">
         <v>99.2</v>
@@ -1052,7 +1055,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4">
         <v>635.29999999999995</v>
@@ -1087,7 +1090,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>1011.7</v>
@@ -1122,7 +1125,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4">
         <v>45</v>
@@ -1157,7 +1160,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4">
         <v>731.5</v>
@@ -1192,7 +1195,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4">
         <v>8.4</v>
@@ -1227,7 +1230,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4">
         <v>27</v>
@@ -1262,7 +1265,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4">
         <v>24</v>
@@ -1297,7 +1300,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4">
         <v>9.1</v>
@@ -1332,7 +1335,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>186.1</v>
@@ -1367,7 +1370,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4">
         <v>8.1999999999999993</v>
@@ -1402,7 +1405,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4">
         <v>326.39999999999998</v>
@@ -1437,7 +1440,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4">
         <v>146.30000000000001</v>
@@ -1472,7 +1475,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4">
         <v>411.9</v>
@@ -1507,7 +1510,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4">
         <v>109.7</v>
@@ -1542,7 +1545,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="4">
         <v>155.1</v>
@@ -1577,7 +1580,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4">
         <v>48.6</v>
@@ -1612,7 +1615,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>88.2</v>
@@ -1647,7 +1650,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>144.30000000000001</v>
@@ -1682,7 +1685,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4">
         <v>218.4</v>
@@ -1717,7 +1720,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>1215.5999999999999</v>
@@ -1752,7 +1755,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4">
         <v>8.1999999999999993</v>
@@ -1787,7 +1790,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
         <v>92.3</v>
@@ -1822,7 +1825,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="4">
         <v>229.6</v>
@@ -1857,10 +1860,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="4">
         <v>4.9000000000000004</v>
@@ -1892,10 +1895,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4">
         <v>12.2</v>
@@ -1927,7 +1930,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="4">
         <v>58.4</v>
@@ -1962,7 +1965,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4">
         <v>242.6</v>
@@ -2013,9 +2016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23699C2B-F43B-4CFB-984B-EEFACA49789A}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="A41:C43"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2025,42 +2026,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>498.4</v>
@@ -2095,7 +2096,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>594.70000000000005</v>
@@ -2130,7 +2131,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>548.1</v>
@@ -2165,7 +2166,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>431.8</v>
@@ -2200,7 +2201,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>15.1</v>
@@ -2235,34 +2236,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7" s="4">
         <v>3</v>
@@ -2270,7 +2271,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4">
         <v>5.0999999999999996</v>
@@ -2305,7 +2306,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
         <v>18.899999999999999</v>
@@ -2340,7 +2341,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4">
         <v>101.3</v>
@@ -2375,13 +2376,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4">
         <v>1.1000000000000001</v>
@@ -2390,27 +2391,27 @@
         <v>1.5</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" s="4">
         <v>1.4</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="4">
         <v>1</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>8.6</v>
@@ -2445,7 +2446,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4">
         <v>5.8</v>
@@ -2480,7 +2481,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4">
         <v>58.1</v>
@@ -2515,7 +2516,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>92.5</v>
@@ -2550,10 +2551,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="4">
         <v>1.4</v>
@@ -2565,7 +2566,7 @@
         <v>1.6</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="4">
         <v>1.3</v>
@@ -2577,15 +2578,15 @@
         <v>1</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4">
         <v>67</v>
@@ -2620,112 +2621,112 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4">
         <v>1.3</v>
@@ -2760,7 +2761,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>14.6</v>
@@ -2795,7 +2796,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4">
         <v>3.2</v>
@@ -2830,7 +2831,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4">
         <v>28.7</v>
@@ -2865,7 +2866,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4">
         <v>11.1</v>
@@ -2900,7 +2901,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4">
         <v>7.9</v>
@@ -2915,7 +2916,7 @@
         <v>5.9</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G26" s="4">
         <v>9.1</v>
@@ -2927,15 +2928,15 @@
         <v>5.7</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4">
         <v>26.2</v>
@@ -2970,10 +2971,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="4">
         <v>8.3000000000000007</v>
@@ -3000,12 +3001,12 @@
         <v>7.8</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4">
         <v>2.2999999999999998</v>
@@ -3040,7 +3041,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>2.2999999999999998</v>
@@ -3049,19 +3050,19 @@
         <v>2.1</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I30" s="4">
         <v>4.0999999999999996</v>
@@ -3070,12 +3071,12 @@
         <v>3.1</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>6.2</v>
@@ -3110,7 +3111,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4">
         <v>11.2</v>
@@ -3145,7 +3146,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>96.3</v>
@@ -3180,7 +3181,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4">
         <v>1.4</v>
@@ -3215,7 +3216,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
         <v>8.3000000000000007</v>
@@ -3250,7 +3251,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="4">
         <v>24.7</v>
@@ -3285,69 +3286,69 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H38" s="4">
         <v>0.5</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K38" s="4">
         <v>0.8</v>
@@ -3355,16 +3356,16 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="4">
         <v>3.4</v>
@@ -3373,16 +3374,16 @@
         <v>1.6</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I39" s="4">
         <v>1.1000000000000001</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K39" s="4">
         <v>1.5</v>
@@ -3390,7 +3391,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4">
         <v>58.1</v>
@@ -3442,7 +3443,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3453,42 +3454,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>2808.9</v>
@@ -3523,7 +3524,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>3189</v>
@@ -3558,7 +3559,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>2540.5</v>
@@ -3593,7 +3594,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>2120.5</v>
@@ -3628,7 +3629,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>52.3</v>
@@ -3663,7 +3664,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>42.3</v>
@@ -3698,7 +3699,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4">
         <v>125.3</v>
@@ -3733,7 +3734,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
         <v>55.2</v>
@@ -3768,7 +3769,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4">
         <v>792.8</v>
@@ -3803,7 +3804,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4">
         <v>7.9</v>
@@ -3838,7 +3839,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>35</v>
@@ -3873,7 +3874,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4">
         <v>43.1</v>
@@ -3908,7 +3909,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4">
         <v>122.8</v>
@@ -3943,7 +3944,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>260</v>
@@ -3978,7 +3979,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4">
         <v>21.2</v>
@@ -4013,7 +4014,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4">
         <v>423.3</v>
@@ -4048,7 +4049,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4">
         <v>2.6</v>
@@ -4083,7 +4084,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4">
         <v>10.7</v>
@@ -4118,7 +4119,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4">
         <v>5.6</v>
@@ -4153,7 +4154,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4">
         <v>3.2</v>
@@ -4188,7 +4189,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>105.8</v>
@@ -4223,7 +4224,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4">
         <v>2.5</v>
@@ -4258,7 +4259,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4">
         <v>114.1</v>
@@ -4293,7 +4294,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4">
         <v>87.1</v>
@@ -4328,7 +4329,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4">
         <v>173.9</v>
@@ -4363,7 +4364,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4">
         <v>37</v>
@@ -4398,7 +4399,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="4">
         <v>76.3</v>
@@ -4433,7 +4434,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4">
         <v>25.7</v>
@@ -4468,7 +4469,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>48.6</v>
@@ -4503,7 +4504,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>46.1</v>
@@ -4538,7 +4539,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4">
         <v>88.5</v>
@@ -4573,7 +4574,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>380.1</v>
@@ -4608,7 +4609,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4">
         <v>2.5</v>
@@ -4643,7 +4644,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
         <v>26.9</v>
@@ -4678,7 +4679,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="4">
         <v>95.7</v>
@@ -4713,10 +4714,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="4">
         <v>2.7</v>
@@ -4748,10 +4749,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4">
         <v>7.7</v>
@@ -4783,7 +4784,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="4">
         <v>32</v>
@@ -4818,7 +4819,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4">
         <v>85.7</v>
@@ -4869,8 +4870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2B16F5-5697-4DE0-9945-AA35F370E5EC}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="A41:C43"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4881,42 +4882,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>3569.7</v>
@@ -4951,7 +4952,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>4300.6000000000004</v>
@@ -4986,7 +4987,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>3671</v>
@@ -5021,7 +5022,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>2864</v>
@@ -5056,7 +5057,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>143.80000000000001</v>
@@ -5091,7 +5092,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>48.6</v>
@@ -5126,7 +5127,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4">
         <v>78.900000000000006</v>
@@ -5161,7 +5162,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
         <v>67.900000000000006</v>
@@ -5196,7 +5197,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4">
         <v>732.4</v>
@@ -5231,7 +5232,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4">
         <v>10.8</v>
@@ -5266,7 +5267,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>99.6</v>
@@ -5301,7 +5302,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4">
         <v>50.3</v>
@@ -5336,7 +5337,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4">
         <v>454.4</v>
@@ -5371,7 +5372,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>659.3</v>
@@ -5406,7 +5407,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4">
         <v>23</v>
@@ -5441,7 +5442,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4">
         <v>241.2</v>
@@ -5476,7 +5477,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4">
         <v>5.3</v>
@@ -5511,7 +5512,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4">
         <v>15.5</v>
@@ -5546,7 +5547,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4">
         <v>18.2</v>
@@ -5581,7 +5582,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4">
         <v>4.3</v>
@@ -5616,7 +5617,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>65.8</v>
@@ -5651,7 +5652,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4">
         <v>2.5</v>
@@ -5686,7 +5687,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4">
         <v>182</v>
@@ -5721,7 +5722,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4">
         <v>48.1</v>
@@ -5756,7 +5757,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4">
         <v>230.2</v>
@@ -5791,7 +5792,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4">
         <v>46.5</v>
@@ -5826,7 +5827,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="4">
         <v>73</v>
@@ -5861,7 +5862,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4">
         <v>20.5</v>
@@ -5896,7 +5897,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>37.299999999999997</v>
@@ -5931,7 +5932,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>92</v>
@@ -5966,7 +5967,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4">
         <v>118.4</v>
@@ -6001,7 +6002,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>730.9</v>
@@ -6036,7 +6037,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4">
         <v>4.3</v>
@@ -6071,7 +6072,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
         <v>57.1</v>
@@ -6106,7 +6107,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="4">
         <v>108.6</v>
@@ -6141,10 +6142,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="4">
         <v>2</v>
@@ -6176,10 +6177,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4">
         <v>4</v>
@@ -6211,7 +6212,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="4">
         <v>24.9</v>
@@ -6246,7 +6247,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4">
         <v>98.8</v>
@@ -6297,8 +6298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990017F1-864E-402B-A1F0-657F9FFF933A}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="A41:C43"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6309,42 +6310,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>7.2</v>
@@ -6379,7 +6380,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>7.3</v>
@@ -6414,7 +6415,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>8.1</v>
@@ -6449,7 +6450,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>8</v>
@@ -6484,7 +6485,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>7.1</v>
@@ -6519,34 +6520,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7" s="4">
         <v>2.2999999999999998</v>
@@ -6554,7 +6555,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4">
         <v>2.4</v>
@@ -6589,7 +6590,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
         <v>13</v>
@@ -6624,7 +6625,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4">
         <v>6.2</v>
@@ -6659,13 +6660,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4">
         <v>5</v>
@@ -6674,27 +6675,27 @@
         <v>5.7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" s="4">
         <v>3.9</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="4">
         <v>2.8</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>5.9</v>
@@ -6729,7 +6730,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4">
         <v>5.9</v>
@@ -6764,7 +6765,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4">
         <v>9.1</v>
@@ -6799,7 +6800,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>9.1</v>
@@ -6834,10 +6835,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="4">
         <v>3.2</v>
@@ -6849,7 +6850,7 @@
         <v>3.9</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="4">
         <v>2.5</v>
@@ -6861,15 +6862,15 @@
         <v>1.8</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4">
         <v>9.1999999999999993</v>
@@ -6904,112 +6905,112 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4">
         <v>13.9</v>
@@ -7044,7 +7045,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>7.8</v>
@@ -7079,7 +7080,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4">
         <v>39.299999999999997</v>
@@ -7114,7 +7115,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4">
         <v>8.8000000000000007</v>
@@ -7149,7 +7150,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4">
         <v>7.6</v>
@@ -7184,7 +7185,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4">
         <v>1.9</v>
@@ -7199,7 +7200,7 @@
         <v>1.3</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G26" s="4">
         <v>1.9</v>
@@ -7211,15 +7212,15 @@
         <v>1.2</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4">
         <v>23.9</v>
@@ -7254,10 +7255,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="4">
         <v>4.8</v>
@@ -7284,12 +7285,12 @@
         <v>3</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4">
         <v>4.8</v>
@@ -7324,7 +7325,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>2.6</v>
@@ -7333,19 +7334,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I30" s="4">
         <v>3.7</v>
@@ -7354,12 +7355,12 @@
         <v>2.8</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>4.3</v>
@@ -7394,7 +7395,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4">
         <v>5.0999999999999996</v>
@@ -7429,7 +7430,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>7.9</v>
@@ -7464,7 +7465,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4">
         <v>16.899999999999999</v>
@@ -7499,7 +7500,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
         <v>9</v>
@@ -7534,7 +7535,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="4">
         <v>10.7</v>
@@ -7569,69 +7570,69 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H38" s="4">
         <v>3.4</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K38" s="4">
         <v>3.9</v>
@@ -7639,16 +7640,16 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="4">
         <v>5.7</v>
@@ -7657,16 +7658,16 @@
         <v>2.4</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I39" s="4">
         <v>1.3</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K39" s="4">
         <v>1.5</v>
@@ -7674,7 +7675,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4">
         <v>24</v>
@@ -7725,8 +7726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B934C1F-0AC1-4EC2-801B-7AC682FA8804}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="A41:C43"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7737,42 +7738,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>40.799999999999997</v>
@@ -7807,7 +7808,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>39.4</v>
@@ -7842,7 +7843,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>37.5</v>
@@ -7877,7 +7878,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>39.1</v>
@@ -7912,7 +7913,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>24.7</v>
@@ -7947,7 +7948,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>45.3</v>
@@ -7982,7 +7983,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4">
         <v>59.8</v>
@@ -8017,7 +8018,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
         <v>38.200000000000003</v>
@@ -8052,7 +8053,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4">
         <v>48.7</v>
@@ -8087,7 +8088,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4">
         <v>40.700000000000003</v>
@@ -8122,7 +8123,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>23.8</v>
@@ -8157,7 +8158,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4">
         <v>43.4</v>
@@ -8192,7 +8193,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4">
         <v>19.3</v>
@@ -8227,7 +8228,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>25.7</v>
@@ -8262,7 +8263,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4">
         <v>47.2</v>
@@ -8297,7 +8298,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4">
         <v>57.9</v>
@@ -8332,7 +8333,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4">
         <v>31.3</v>
@@ -8367,7 +8368,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4">
         <v>39.700000000000003</v>
@@ -8402,7 +8403,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4">
         <v>23.5</v>
@@ -8437,7 +8438,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4">
         <v>35.1</v>
@@ -8472,7 +8473,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>56.8</v>
@@ -8507,7 +8508,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4">
         <v>30.2</v>
@@ -8542,7 +8543,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4">
         <v>35</v>
@@ -8577,7 +8578,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4">
         <v>59.5</v>
@@ -8612,7 +8613,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4">
         <v>42.2</v>
@@ -8647,7 +8648,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4">
         <v>33.799999999999997</v>
@@ -8682,7 +8683,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="4">
         <v>49.2</v>
@@ -8717,7 +8718,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4">
         <v>52.9</v>
@@ -8752,7 +8753,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>55.1</v>
@@ -8787,7 +8788,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>31.9</v>
@@ -8822,7 +8823,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4">
         <v>40.5</v>
@@ -8857,7 +8858,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>31.3</v>
@@ -8892,7 +8893,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4">
         <v>30</v>
@@ -8927,7 +8928,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
         <v>29.2</v>
@@ -8962,7 +8963,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="4">
         <v>41.7</v>
@@ -8997,10 +8998,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="4">
         <v>56.3</v>
@@ -9032,10 +9033,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4">
         <v>63.3</v>
@@ -9067,7 +9068,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="4">
         <v>54.8</v>
@@ -9102,7 +9103,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4">
         <v>35.299999999999997</v>
@@ -9154,7 +9155,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -9165,42 +9166,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>51.8</v>
@@ -9235,7 +9236,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>53.1</v>
@@ -9270,7 +9271,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>54.2</v>
@@ -9305,7 +9306,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>52.8</v>
@@ -9340,7 +9341,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>68.099999999999994</v>
@@ -9375,7 +9376,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>52.1</v>
@@ -9410,7 +9411,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4">
         <v>37.700000000000003</v>
@@ -9445,7 +9446,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
         <v>47</v>
@@ -9480,7 +9481,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4">
         <v>45</v>
@@ -9515,7 +9516,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4">
         <v>55.4</v>
@@ -9550,7 +9551,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>67.8</v>
@@ -9585,7 +9586,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4">
         <v>50.7</v>
@@ -9620,7 +9621,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4">
         <v>71.5</v>
@@ -9655,7 +9656,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>65.2</v>
@@ -9690,7 +9691,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4">
         <v>51.2</v>
@@ -9725,7 +9726,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4">
         <v>33</v>
@@ -9760,7 +9761,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4">
         <v>63</v>
@@ -9795,7 +9796,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4">
         <v>57.4</v>
@@ -9830,7 +9831,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4">
         <v>76</v>
@@ -9865,7 +9866,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4">
         <v>47.7</v>
@@ -9900,7 +9901,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>35.299999999999997</v>
@@ -9935,7 +9936,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4">
         <v>30.5</v>
@@ -9970,7 +9971,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4">
         <v>55.8</v>
@@ -10005,7 +10006,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4">
         <v>32.9</v>
@@ -10040,7 +10041,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4">
         <v>55.9</v>
@@ -10075,7 +10076,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4">
         <v>42.4</v>
@@ -10110,7 +10111,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="4">
         <v>47.1</v>
@@ -10145,7 +10146,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4">
         <v>42.3</v>
@@ -10180,7 +10181,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>42.2</v>
@@ -10215,7 +10216,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>63.8</v>
@@ -10250,7 +10251,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4">
         <v>54.2</v>
@@ -10285,7 +10286,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>60.1</v>
@@ -10320,7 +10321,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4">
         <v>53</v>
@@ -10355,7 +10356,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
         <v>61.9</v>
@@ -10390,7 +10391,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="4">
         <v>47.3</v>
@@ -10425,10 +10426,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="4">
         <v>40.200000000000003</v>
@@ -10460,10 +10461,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4">
         <v>33.1</v>
@@ -10495,7 +10496,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="4">
         <v>42.7</v>
@@ -10530,7 +10531,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4">
         <v>40.700000000000003</v>

</xml_diff>